<commit_message>
Added files for Calendar year 2017
</commit_message>
<xml_diff>
--- a/UK-Sales_Predictive_Model/2016/6. LM with Weather + Lasso/Output_Data/Lasso_Weather_Output_Analyzed.xlsx
+++ b/UK-Sales_Predictive_Model/2016/6. LM with Weather + Lasso/Output_Data/Lasso_Weather_Output_Analyzed.xlsx
@@ -15,9 +15,9 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Lasso_Weather_Output!$A$3:$H$158</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="9" r:id="rId3"/>
+    <pivotCache cacheId="10" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -1105,13 +1105,7 @@
     <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
@@ -4882,7 +4876,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="M6:N18" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="10">
     <pivotField showAll="0"/>
@@ -5122,7 +5116,7 @@
     <dataField name="Sum of USD Avg. Store Daily Sales" fld="9" baseField="4" baseItem="0" numFmtId="44"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="2">
+    <format dxfId="0">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -5425,7 +5419,7 @@
   <dimension ref="A2:N158"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added average values to the lasso output file
</commit_message>
<xml_diff>
--- a/UK-Sales_Predictive_Model/2016/6. LM with Weather + Lasso/Output_Data/Lasso_Weather_Output_Analyzed.xlsx
+++ b/UK-Sales_Predictive_Model/2016/6. LM with Weather + Lasso/Output_Data/Lasso_Weather_Output_Analyzed.xlsx
@@ -17,7 +17,7 @@
   </definedNames>
   <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="10" r:id="rId3"/>
+    <pivotCache cacheId="11" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -4876,7 +4876,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="M6:N18" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="10">
     <pivotField showAll="0"/>
@@ -5416,10 +5416,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A2:N158"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="F168" sqref="F168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5436,6 +5437,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0.72127988066314097</v>
+      </c>
+      <c r="B2">
+        <v>0.71229736846149805</v>
+      </c>
+      <c r="C2">
+        <v>0.64156102424362205</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
       <c r="H2">
         <f>SUM(H5:H158)</f>
         <v>8617.8788631283005</v>
@@ -5476,19 +5489,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>0.72127988066314097</v>
-      </c>
-      <c r="B4">
-        <v>0.71229736846149805</v>
-      </c>
-      <c r="C4">
-        <v>0.64156102424362205</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
+    <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="M4" s="4" t="s">
         <v>3</v>
       </c>
@@ -5617,7 +5618,7 @@
         <v>34.250830620064121</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>-16.477516692015001</v>
       </c>
@@ -5659,7 +5660,7 @@
         <v>-40.181832199295208</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>-22.985450075717399</v>
       </c>
@@ -5701,7 +5702,7 @@
         <v>45.024359319442723</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2.9746881312931399</v>
       </c>
@@ -5743,7 +5744,7 @@
         <v>205.14875032380684</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>-0.14465014805496801</v>
       </c>
@@ -5785,7 +5786,7 @@
         <v>0.91444096496464211</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>-2.3329108803235901</v>
       </c>
@@ -5827,7 +5828,7 @@
         <v>22.630479785992289</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>-0.80056403163642997</v>
       </c>
@@ -5869,7 +5870,7 @@
         <v>149.93143780623893</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>0</v>
       </c>
@@ -5911,7 +5912,7 @@
         <v>48.145589252023363</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>10.7521132270042</v>
       </c>
@@ -5953,7 +5954,7 @@
         <v>1.1706674647834023</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>346.84485271778698</v>
       </c>
@@ -5995,7 +5996,7 @@
         <v>759.44061540547386</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>-67.6274803883815</v>
       </c>
@@ -6037,7 +6038,7 @@
         <v>3.1193372565048367</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>448.48771538098299</v>
       </c>
@@ -6079,7 +6080,7 @@
         <v>1229.5946759999997</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>652.35962208456499</v>
       </c>
@@ -6115,7 +6116,7 @@
         <v>93.078346875413843</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>-1194.4303148128799</v>
       </c>
@@ -6151,7 +6152,7 @@
         <v>-170.420724086831</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>-730.10764775569999</v>
       </c>
@@ -6187,7 +6188,7 @@
         <v>-104.17139656351732</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>-113.228849499422</v>
       </c>
@@ -6223,7 +6224,7 @@
         <v>-16.155436009871632</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>0</v>
       </c>
@@ -6259,7 +6260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>-199.949981811241</v>
       </c>
@@ -6295,7 +6296,7 @@
         <v>-28.528764096847866</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>-5.4872025754407696</v>
       </c>
@@ -6331,7 +6332,7 @@
         <v>-0.78291133816729885</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>0</v>
       </c>
@@ -6367,7 +6368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>-181.261992596439</v>
       </c>
@@ -6403,7 +6404,7 @@
         <v>-25.862371077333471</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>0</v>
       </c>
@@ -6439,7 +6440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>-35.910071253042098</v>
       </c>
@@ -6475,7 +6476,7 @@
         <v>-5.1236311311404243</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>58.249053221182699</v>
       </c>
@@ -6511,7 +6512,7 @@
         <v>8.3109459833841015</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>0</v>
       </c>
@@ -6547,7 +6548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>0</v>
       </c>
@@ -6583,7 +6584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>16.1524484166486</v>
       </c>
@@ -6619,7 +6620,7 @@
         <v>2.3046233177459858</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>68.338701327656395</v>
       </c>
@@ -6655,7 +6656,7 @@
         <v>9.7505319640496602</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>26.573298805131799</v>
       </c>
@@ -6691,7 +6692,7 @@
         <v>3.7914650755123724</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>432.34050092516401</v>
       </c>
@@ -6727,7 +6728,7 @@
         <v>61.686127943991778</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>-105.805823074586</v>
       </c>
@@ -6763,7 +6764,7 @@
         <v>-15.096322286326853</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>0</v>
       </c>
@@ -6799,7 +6800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>-1261.5691547486499</v>
       </c>
@@ -6835,7 +6836,7 @@
         <v>-180.0000604234144</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>0</v>
       </c>
@@ -6871,7 +6872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>-24.222814753851601</v>
       </c>
@@ -6907,7 +6908,7 @@
         <v>-3.4560991784767863</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>-49.915974226091002</v>
       </c>
@@ -6943,7 +6944,7 @@
         <v>-7.1219864111056905</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>-93.229280415797803</v>
       </c>
@@ -6979,7 +6980,7 @@
         <v>-13.301907426088334</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>42.582461788996802</v>
       </c>
@@ -7015,7 +7016,7 @@
         <v>6.075644498873527</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>-43.1187461965865</v>
       </c>
@@ -7051,7 +7052,7 @@
         <v>-6.1521612917952062</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>232.47669448634099</v>
       </c>
@@ -7087,7 +7088,7 @@
         <v>33.169659306480291</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>0</v>
       </c>
@@ -7123,7 +7124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>0</v>
       </c>
@@ -7159,7 +7160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>29.1924215466981</v>
       </c>
@@ -7195,7 +7196,7 @@
         <v>4.1651602074547842</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>0</v>
       </c>
@@ -7231,7 +7232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>454.87062038878003</v>
       </c>
@@ -7267,7 +7268,7 @@
         <v>64.900714199158742</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>401.74499867507802</v>
       </c>
@@ -7303,7 +7304,7 @@
         <v>57.320776878637432</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>-16.1875191218375</v>
       </c>
@@ -7339,7 +7340,7 @@
         <v>-2.3096271885439772</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>-249.547309536895</v>
       </c>
@@ -7375,7 +7376,7 @@
         <v>-35.605286183531483</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>482.01498211585999</v>
       </c>
@@ -7411,7 +7412,7 @@
         <v>68.77365824874822</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>616.25264722479403</v>
       </c>
@@ -7447,7 +7448,7 @@
         <v>87.926621635460307</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>0</v>
       </c>
@@ -7483,7 +7484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>0</v>
       </c>
@@ -7519,7 +7520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>103.403482616779</v>
       </c>
@@ -7555,7 +7556,7 @@
         <v>14.753557542963238</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>-50.0667487884132</v>
       </c>
@@ -7591,7 +7592,7 @@
         <v>-7.1434988507735078</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>12.731603288890099</v>
       </c>
@@ -7627,7 +7628,7 @@
         <v>1.8165388339284079</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>37.571417729202501</v>
       </c>
@@ -7663,7 +7664,7 @@
         <v>5.36067122122782</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>-280.20219332179801</v>
       </c>
@@ -7699,7 +7700,7 @@
         <v>-39.979109776780838</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>-22.005911863887601</v>
       </c>
@@ -7735,7 +7736,7 @@
         <v>-3.1397925751928262</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>-48.6910312130953</v>
       </c>
@@ -7771,7 +7772,7 @@
         <v>-6.9472121503966973</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>54.0358253825205</v>
       </c>
@@ -7807,7 +7808,7 @@
         <v>7.7098047279228386</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>595.26132287197504</v>
       </c>
@@ -7843,7 +7844,7 @@
         <v>84.931589902437551</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>0</v>
       </c>
@@ -7879,7 +7880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>64.672308158911207</v>
       </c>
@@ -7915,7 +7916,7 @@
         <v>9.2274128076990003</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>-235.19117021945499</v>
       </c>
@@ -7951,7 +7952,7 @@
         <v>-33.556959355898321</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>131.022286982331</v>
       </c>
@@ -7987,7 +7988,7 @@
         <v>18.694194832571277</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>-57.883207180501003</v>
       </c>
@@ -8023,7 +8024,7 @@
         <v>-8.2587472520022356</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>-138.77441809336401</v>
       </c>
@@ -8059,7 +8060,7 @@
         <v>-19.800265049288157</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>45.0940511472837</v>
       </c>
@@ -8095,7 +8096,7 @@
         <v>6.4339968210976046</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>0</v>
       </c>
@@ -8131,7 +8132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>-3.8287178060748399</v>
       </c>
@@ -8167,7 +8168,7 @@
         <v>-0.54627955498403202</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>37.225039321775</v>
       </c>
@@ -8203,7 +8204,7 @@
         <v>5.3112501220897883</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>-103.868451285841</v>
       </c>
@@ -8239,7 +8240,7 @@
         <v>-14.819899041731755</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>-8.0607288572841806</v>
       </c>
@@ -8275,7 +8276,7 @@
         <v>-1.1501007898825735</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>6.4090562665606701</v>
       </c>
@@ -8311,7 +8312,7 @@
         <v>0.91444096496464211</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>88.1367940489462</v>
       </c>
@@ -8347,7 +8348,7 @@
         <v>12.575314000521164</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>240.054316277178</v>
       </c>
@@ -8383,7 +8384,7 @@
         <v>34.250830620064121</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>0</v>
       </c>
@@ -8419,7 +8420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>-26.336902909148499</v>
       </c>
@@ -8455,7 +8456,7 @@
         <v>-3.7577362264828329</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>36.708910092607901</v>
       </c>
@@ -8491,7 +8492,7 @@
         <v>5.2376090600150915</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>-11.7710677812473</v>
       </c>
@@ -8527,7 +8528,7 @@
         <v>-1.6794901047614474</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>348.323775026796</v>
       </c>
@@ -8563,7 +8564,7 @@
         <v>49.698663220905118</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>-33.203557589699898</v>
       </c>
@@ -8599,7 +8600,7 @@
         <v>-4.7374671058829625</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>0</v>
       </c>
@@ -8635,7 +8636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>86.443324865608204</v>
       </c>
@@ -8671,7 +8672,7 @@
         <v>12.333690658527864</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>17.2680576535444</v>
       </c>
@@ -8707,7 +8708,7 @@
         <v>2.4637978895832084</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>-10.957253986382799</v>
       </c>
@@ -8743,7 +8744,7 @@
         <v>-1.5633755567022856</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>0</v>
       </c>
@@ -8779,7 +8780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>-92.311435623530599</v>
       </c>
@@ -9031,7 +9032,7 @@
         <v>-5.2889521411999514</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>0</v>
       </c>
@@ -9211,7 +9212,7 @@
         <v>73.870158373862353</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>-59.792679743131899</v>
       </c>
@@ -9247,7 +9248,7 @@
         <v>-8.5311898488719198</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>-83.723307906909099</v>
       </c>
@@ -9283,7 +9284,7 @@
         <v>-11.945599989795483</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>-68.700098326836795</v>
       </c>
@@ -9319,7 +9320,7 @@
         <v>-9.8020959083997976</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>-41.993627132856197</v>
       </c>
@@ -9355,7 +9356,7 @@
         <v>-5.9916298625884261</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>-83.3427711087961</v>
       </c>
@@ -9391,7 +9392,7 @@
         <v>-11.891305188439691</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>-378.621184600314</v>
       </c>
@@ -9427,7 +9428,7 @@
         <v>-54.021482571218662</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>-286.425902324481</v>
       </c>
@@ -9463,7 +9464,7 @@
         <v>-40.867105486190745</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>-66.235165598443501</v>
       </c>
@@ -9499,7 +9500,7 @@
         <v>-9.4504005309562658</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>-107.955287396616</v>
       </c>
@@ -9535,7 +9536,7 @@
         <v>-15.403006788232306</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>-255.990415584158</v>
       </c>
@@ -9571,7 +9572,7 @@
         <v>-36.524585354295432</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>-199.38860563557401</v>
       </c>
@@ -9607,7 +9608,7 @@
         <v>-28.448667222919099</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>-119.75064887383</v>
       </c>
@@ -9643,7 +9644,7 @@
         <v>-17.085963105468476</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>-431.43042704432099</v>
       </c>
@@ -9679,7 +9680,7 @@
         <v>-61.556279054674128</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>-116.702166795271</v>
       </c>
@@ -9715,7 +9716,7 @@
         <v>-16.651007196571317</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>-228.87796688263899</v>
       </c>
@@ -9751,7 +9752,7 @@
         <v>-32.656194639342935</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>-96.9261085036065</v>
       </c>
@@ -9787,7 +9788,7 @@
         <v>-13.829369021575042</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>4.9559186047527799</v>
       </c>
@@ -9823,7 +9824,7 @@
         <v>0.70710800509921767</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>-143.762934233057</v>
       </c>
@@ -9859,7 +9860,7 @@
         <v>-20.51202405448262</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>-74.734861707667605</v>
       </c>
@@ -9895,7 +9896,7 @@
         <v>-10.663132950326348</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>0</v>
       </c>
@@ -9931,7 +9932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>109.38215179948099</v>
       </c>
@@ -9967,7 +9968,7 @@
         <v>15.606591092560743</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>123.296900292237</v>
       </c>
@@ -10003,7 +10004,7 @@
         <v>17.591940496550976</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>105.42741137616299</v>
       </c>
@@ -10039,7 +10040,7 @@
         <v>15.042330693139368</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>136.18913761027099</v>
       </c>
@@ -10075,7 +10076,7 @@
         <v>19.431398513976479</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>122.88591064034701</v>
       </c>
@@ -10111,7 +10112,7 @@
         <v>17.533300697143122</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>95.343020208663603</v>
       </c>
@@ -10147,7 +10148,7 @@
         <v>13.603494769915732</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>0</v>
       </c>
@@ -10183,7 +10184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>-6.8307969471906098</v>
       </c>
@@ -10219,7 +10220,7 @@
         <v>-0.9746147158134616</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>0</v>
       </c>
@@ -10255,7 +10256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>181.671970490527</v>
       </c>
@@ -10291,7 +10292,7 @@
         <v>25.92086651964064</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>19.871659850949801</v>
       </c>
@@ -10327,7 +10328,7 @@
         <v>2.8352785579932394</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>-108.979011240425</v>
       </c>
@@ -10363,7 +10364,7 @@
         <v>-15.54907119782008</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>-103.913139463631</v>
       </c>
@@ -10399,7 +10400,7 @@
         <v>-14.826275128743818</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>-44.4872416786435</v>
       </c>
@@ -10435,7 +10436,7 @@
         <v>-6.3474175474925074</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>49.056650391423297</v>
       </c>
@@ -10471,7 +10472,7 @@
         <v>6.999378513170611</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>118.606089678149</v>
       </c>
@@ -10507,7 +10508,7 @@
         <v>16.922657967890189</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>98.052100032414899</v>
       </c>
@@ -10543,7 +10544,7 @@
         <v>13.990024933665845</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>94.329683899158198</v>
       </c>
@@ -10579,7 +10580,7 @@
         <v>13.458912448563279</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>64.075517673689504</v>
       </c>
@@ -10615,7 +10616,7 @@
         <v>9.1422630376719827</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>48.472201252597998</v>
       </c>
@@ -10651,7 +10652,7 @@
         <v>6.9159896003179293</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>-82.128837903615505</v>
       </c>
@@ -10687,7 +10688,7 @@
         <v>-11.718101801641579</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>-121.271571843899</v>
       </c>
@@ -10723,7 +10724,7 @@
         <v>-17.302967639450067</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>682.40061541961097</v>
       </c>
@@ -10759,7 +10760,7 @@
         <v>97.364580884174956</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>85.824189762175706</v>
       </c>
@@ -10795,7 +10796,7 @@
         <v>12.245352769472301</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>174.67306196982199</v>
       </c>
@@ -10831,7 +10832,7 @@
         <v>24.922265728013127</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>282.168938309456</v>
       </c>
@@ -10867,7 +10868,7 @@
         <v>40.259723974808225</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>434.39080571397801</v>
       </c>
@@ -10903,7 +10904,7 @@
         <v>61.978664412946955</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>609.86936912383101</v>
       </c>
@@ -10939,7 +10940,7 @@
         <v>87.015858686360033</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>877.89975233713403</v>
       </c>
@@ -10975,7 +10976,7 @@
         <v>125.25830064216207</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>1196.7437032869</v>
       </c>
@@ -11011,7 +11012,7 @@
         <v>170.75079720532716</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>1816.7313780109801</v>
       </c>
@@ -11047,7 +11048,7 @@
         <v>259.21033070933146</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>1441.18947365335</v>
       </c>
@@ -11083,7 +11084,7 @@
         <v>205.62819831377098</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>-338.83988822886602</v>
       </c>
@@ -11120,7 +11121,150 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:H158"/>
+  <autoFilter ref="A3:H158">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="0.070110385"/>
+        <filter val="-0.144650148"/>
+        <filter val="0.721279881"/>
+        <filter val="-0.800564032"/>
+        <filter val="10.75211323"/>
+        <filter val="-10.95725399"/>
+        <filter val="103.4034826"/>
+        <filter val="-103.8684513"/>
+        <filter val="-103.9131395"/>
+        <filter val="105.4274114"/>
+        <filter val="-105.8058231"/>
+        <filter val="-107.9552874"/>
+        <filter val="-108.9790112"/>
+        <filter val="109.3821518"/>
+        <filter val="-11.77106778"/>
+        <filter val="-113.2288495"/>
+        <filter val="-116.7021668"/>
+        <filter val="118.6060897"/>
+        <filter val="-119.7506489"/>
+        <filter val="-1194.430315"/>
+        <filter val="1196.743703"/>
+        <filter val="12.73160329"/>
+        <filter val="-121.2715718"/>
+        <filter val="122.8859106"/>
+        <filter val="123.2969003"/>
+        <filter val="-1261.569155"/>
+        <filter val="131.022287"/>
+        <filter val="136.1891376"/>
+        <filter val="-138.7744181"/>
+        <filter val="-143.7629342"/>
+        <filter val="1441.189474"/>
+        <filter val="145.4567465"/>
+        <filter val="16.15244842"/>
+        <filter val="-16.18751912"/>
+        <filter val="-16.47751669"/>
+        <filter val="-164.5552037"/>
+        <filter val="17.26805765"/>
+        <filter val="174.673062"/>
+        <filter val="-181.2619926"/>
+        <filter val="181.6719705"/>
+        <filter val="1816.731378"/>
+        <filter val="19.87165985"/>
+        <filter val="-199.3886056"/>
+        <filter val="-199.9499818"/>
+        <filter val="-2.33291088"/>
+        <filter val="2.974688131"/>
+        <filter val="-22.00591186"/>
+        <filter val="-22.98545008"/>
+        <filter val="-228.8779669"/>
+        <filter val="232.4766945"/>
+        <filter val="-235.1911702"/>
+        <filter val="-24.22281475"/>
+        <filter val="240.0543163"/>
+        <filter val="-249.5473095"/>
+        <filter val="-25.05796179"/>
+        <filter val="-255.9904156"/>
+        <filter val="-26.33690291"/>
+        <filter val="26.57329881"/>
+        <filter val="-280.2021933"/>
+        <filter val="282.1689383"/>
+        <filter val="-286.4259023"/>
+        <filter val="29.19242155"/>
+        <filter val="-3.828717806"/>
+        <filter val="-33.20355759"/>
+        <filter val="-338.8398882"/>
+        <filter val="346.8448527"/>
+        <filter val="348.323775"/>
+        <filter val="-35.91007125"/>
+        <filter val="36.70891009"/>
+        <filter val="-37.06875912"/>
+        <filter val="37.22503932"/>
+        <filter val="37.57141773"/>
+        <filter val="-378.6211846"/>
+        <filter val="39.16467435"/>
+        <filter val="4.955918605"/>
+        <filter val="401.7449987"/>
+        <filter val="-41.99362713"/>
+        <filter val="42.58246179"/>
+        <filter val="-43.1187462"/>
+        <filter val="-431.430427"/>
+        <filter val="432.3405009"/>
+        <filter val="434.3908057"/>
+        <filter val="-44.48724168"/>
+        <filter val="446.4453343"/>
+        <filter val="448.4877154"/>
+        <filter val="45.09405115"/>
+        <filter val="-45.53157508"/>
+        <filter val="454.8706204"/>
+        <filter val="48.47220125"/>
+        <filter val="-48.69103121"/>
+        <filter val="482.0149821"/>
+        <filter val="49.05665039"/>
+        <filter val="-49.91597423"/>
+        <filter val="-5.487202575"/>
+        <filter val="-50.06674879"/>
+        <filter val="50.35824915"/>
+        <filter val="517.7348999"/>
+        <filter val="-538.5252962"/>
+        <filter val="54.03582538"/>
+        <filter val="-57.88320718"/>
+        <filter val="58.24905322"/>
+        <filter val="-59.79267974"/>
+        <filter val="595.2613229"/>
+        <filter val="6.409056267"/>
+        <filter val="-6.830796947"/>
+        <filter val="609.8693691"/>
+        <filter val="616.2526472"/>
+        <filter val="64.07551767"/>
+        <filter val="64.67230816"/>
+        <filter val="652.3596221"/>
+        <filter val="-66.2351656"/>
+        <filter val="-67.62748039"/>
+        <filter val="68.33870133"/>
+        <filter val="-68.70009833"/>
+        <filter val="682.4006154"/>
+        <filter val="-7.302279871"/>
+        <filter val="-730.1076478"/>
+        <filter val="-74.73486171"/>
+        <filter val="-8.060728857"/>
+        <filter val="-82.1288379"/>
+        <filter val="-83.34277111"/>
+        <filter val="-83.72330791"/>
+        <filter val="85.82418976"/>
+        <filter val="86.44332487"/>
+        <filter val="864.540127"/>
+        <filter val="877.8997523"/>
+        <filter val="88.13679405"/>
+        <filter val="-92.31143562"/>
+        <filter val="-93.22928042"/>
+        <filter val="94.3296839"/>
+        <filter val="95.34302021"/>
+        <filter val="-96.9261085"/>
+        <filter val="98.05210003"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="5">
+      <filters>
+        <filter val="Base"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>